<commit_message>
added test for default value
</commit_message>
<xml_diff>
--- a/src/test/resources/required.xlsx
+++ b/src/test/resources/required.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="982" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="59">
   <si>
     <t>JOB_ID</t>
   </si>
@@ -147,6 +148,57 @@
   </si>
   <si>
     <t>Public Relations Representative</t>
+  </si>
+  <si>
+    <t>END_DATE</t>
+  </si>
+  <si>
+    <t>START_DATE</t>
+  </si>
+  <si>
+    <t>15.03.05</t>
+  </si>
+  <si>
+    <t>21.09.97</t>
+  </si>
+  <si>
+    <t>28.10.01</t>
+  </si>
+  <si>
+    <t>19.12.07</t>
+  </si>
+  <si>
+    <t>17.02.04</t>
+  </si>
+  <si>
+    <t>31.12.07</t>
+  </si>
+  <si>
+    <t>24.03.06</t>
+  </si>
+  <si>
+    <t>01.01.07</t>
+  </si>
+  <si>
+    <t>17.06.01</t>
+  </si>
+  <si>
+    <t>17.09.95</t>
+  </si>
+  <si>
+    <t>31.12.06</t>
+  </si>
+  <si>
+    <t>01.07.02</t>
+  </si>
+  <si>
+    <t>24.07.06</t>
+  </si>
+  <si>
+    <t>27.10.01</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -262,18 +314,18 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1:E20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -594,18 +646,18 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D25" activeCellId="1" sqref="E1:E20 D25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -901,6 +953,418 @@
         <v>10500</v>
       </c>
       <c r="E20" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.8520408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.219387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="n">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>2008</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>30000</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>6000</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>8200</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>16000</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>4200</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>9000</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>8200</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>16000</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>4200</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>9000</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>20080</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>6000</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>12008</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>15000</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>5500</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>5500</v>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>8500</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>2008</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>5500</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>4000</v>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>9000</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>15000</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>4000</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>9000</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>4500</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>10500</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D22" s="0" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>